<commit_message>
changes in business startup cost
</commit_message>
<xml_diff>
--- a/Documentation/Business-Startup-Cost-v2.xlsx
+++ b/Documentation/Business-Startup-Cost-v2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jana Marie Gardon\Documents\College\4thyr-1st term\Tentrep\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlbel\Desktop\Project---TENTREP\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8508"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="pre" sheetId="1" r:id="rId1"/>
@@ -169,9 +169,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_([$PHP]\ * #,##0_);_([$PHP]\ * \(#,##0\);_([$PHP]\ * &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_([$PHP]\ * #,##0.00_);_([$PHP]\ * \(#,##0.00\);_([$PHP]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$PHP]\ * #,##0_);_([$PHP]\ * \(#,##0\);_([$PHP]\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_([$PHP]\ * #,##0.00_);_([$PHP]\ * \(#,##0.00\);_([$PHP]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -295,7 +295,7 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -309,21 +309,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -345,17 +345,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="4"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="3" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="3" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2"/>
   </cellXfs>
   <cellStyles count="5">
@@ -675,27 +675,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
@@ -709,7 +709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -724,7 +724,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
@@ -738,7 +738,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -753,7 +753,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -768,7 +768,7 @@
         <v>2413</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -783,7 +783,7 @@
         <v>5391.15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
@@ -798,7 +798,7 @@
         <v>7704.63</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
@@ -813,7 +813,7 @@
         <v>8740</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
@@ -828,7 +828,7 @@
         <v>3920</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
@@ -837,13 +837,13 @@
         <v>145168.78</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="5"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>18</v>
       </c>
@@ -860,7 +860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>19</v>
       </c>
@@ -874,7 +874,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
         <v>20</v>
       </c>
@@ -888,7 +888,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
         <v>21</v>
       </c>
@@ -902,7 +902,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
       <c r="D17" s="3"/>
@@ -910,7 +910,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
@@ -927,7 +927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="12" t="s">
         <v>41</v>
@@ -943,7 +943,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="12" t="s">
         <v>43</v>
@@ -959,7 +959,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="12" t="s">
         <v>42</v>
@@ -975,7 +975,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
@@ -985,7 +985,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -994,7 +994,7 @@
         <v>4445.0634</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1003,8 +1003,8 @@
         <v>152613.84340000001</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
         <v>39</v>
       </c>
@@ -1012,11 +1012,11 @@
         <f>(operational!B13*2+(B25))-3000</f>
         <v>2264125.8434000001</v>
       </c>
-      <c r="D28" t="s">
+      <c r="G28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
         <v>36</v>
       </c>
@@ -1024,7 +1024,7 @@
         <f>B25+operational!B13</f>
         <v>1209869.8434000001</v>
       </c>
-      <c r="D29" t="s">
+      <c r="G29" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1038,24 +1038,24 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13" t="s">
         <v>34</v>
@@ -1087,7 +1087,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13" t="s">
         <v>30</v>
@@ -1103,7 +1103,7 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -1113,7 +1113,7 @@
         <v>37250</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="13" t="s">
         <v>32</v>
@@ -1146,7 +1146,7 @@
         <v>180000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="13" t="s">
         <v>33</v>
@@ -1162,7 +1162,7 @@
         <v>360000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="18"/>
@@ -1172,7 +1172,7 @@
         <v>540000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="3" t="s">
         <v>35</v>
@@ -1205,14 +1205,14 @@
         <v>480006</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="3"/>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -1236,9 +1236,9 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3">
         <f>43*100</f>
         <v>4300</v>
@@ -1253,25 +1253,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>2413</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>5391.15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>7704.63</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>8740</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>3920</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
       <c r="D11" s="3"/>
@@ -1413,13 +1413,13 @@
         <v>145168.78</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="5"/>
       <c r="D12" s="3"/>
       <c r="E12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>4</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>3180</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>35</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>3042</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>3078</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>12</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>3513</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="5"/>
       <c r="D19" s="11"/>
@@ -1520,7 +1520,7 @@
         <v>162781.78</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>18</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
         <v>19</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
         <v>20</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
         <v>21</v>
       </c>
@@ -1579,12 +1579,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E25" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>9238.5167999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>317189.07680000004</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <f>2264125.84-operational!E9*(0.05)</f>
         <v>2237125.84</v>

</xml_diff>